<commit_message>
Update to overlay control flow spreadsheet to include aligned interum grids
</commit_message>
<xml_diff>
--- a/NEAP_Extent_DataOverlayMaster.xlsx
+++ b/NEAP_Extent_DataOverlayMaster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/new298_csiro_au/Documents/Code/Python/NEAP/ecosystem-typology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D1C22DC-09ED-456B-B895-6D8CFAADFE82}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D0FB0D4-28F1-460A-83A4-5CFACA69AD55}"/>
   <bookViews>
-    <workbookView xWindow="9012" yWindow="1164" windowWidth="33876" windowHeight="15768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5940" yWindow="420" windowWidth="21600" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -25,29 +25,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
   <si>
     <t>Crosswalk</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
     <t>Crosswalk_comment</t>
   </si>
   <si>
-    <t>Source data</t>
-  </si>
-  <si>
     <t>Resolution</t>
   </si>
   <si>
     <t>Projection</t>
   </si>
   <si>
-    <t>Raster resampling method [nearest neighbour, bi-linear]</t>
-  </si>
-  <si>
     <t>Data_comment</t>
   </si>
   <si>
@@ -135,9 +126,6 @@
     <t>ALUM v8</t>
   </si>
   <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia</t>
-  </si>
-  <si>
     <t>To be updated to latest ALUM when it arrives</t>
   </si>
   <si>
@@ -153,26 +141,68 @@
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\BSU\NEAP_EcoExt_EPSG3577_250m.tif</t>
   </si>
   <si>
-    <t>Vector rasterization method [centre intersect, majority, intersects]</t>
-  </si>
-  <si>
     <t>Input BSU for grid specification</t>
   </si>
   <si>
-    <t>touch</t>
-  </si>
-  <si>
     <t>epsg:4326</t>
   </si>
   <si>
     <t>epsg:4283</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\NLUM_ALUMV8_250m_2010_11_alb\NLUM_ALUMV8_250m_2010_11_alb.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\NLUM_ALUMV8_250m_2015_16_alb\NLUM_ALUMV8_250m_2015_16_alb.tif</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\NEAP_BSU_EPSG3577_250m.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\NEAP_Marine_EPSG3577_250m.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\NEAP_NVIS_EPSG3577_250m.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\NEAP_Esturies_EPSG3577_250m.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\NEAP_Lakes_EPSG3577_250m.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\NEAP_NLUM_2010-11_EPSG3577_250m.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\NEAP_NLUM_2015-16_EPSG3577_250m.tif</t>
+  </si>
+  <si>
+    <t>ALL_TOUCHED</t>
+  </si>
+  <si>
+    <t>RasterResamplingMethod</t>
+  </si>
+  <si>
+    <t>VectorResamplingMethod</t>
+  </si>
+  <si>
+    <t>DataName</t>
+  </si>
+  <si>
+    <t>RawDataPath</t>
+  </si>
+  <si>
+    <t>ResampledRasterPath</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +214,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -206,14 +244,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -492,244 +533,308 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="112.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="125.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" customWidth="1"/>
-    <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="25.44140625" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="112.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="53.42578125" customWidth="1"/>
+    <col min="6" max="6" width="105.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" t="s">
         <v>38</v>
       </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" t="s">
-        <v>43</v>
-      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="H3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="I3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
-        <v>40</v>
+      <c r="J3" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" t="s">
-        <v>40</v>
+      <c r="F5" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="H5" t="s">
         <v>40</v>
       </c>
       <c r="I5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>27</v>
       </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" t="s">
-        <v>37</v>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{240723CA-95A0-4126-A38C-F537203AED46}"/>
+    <hyperlink ref="F5" r:id="rId2" xr:uid="{526F2CB8-0D84-40EB-95F6-0A159D58990C}"/>
+    <hyperlink ref="F6" r:id="rId3" xr:uid="{B35EEF6A-F07D-4114-B04E-E95A54F49F6E}"/>
+    <hyperlink ref="F7" r:id="rId4" xr:uid="{327F660F-B553-4D23-A25D-47C6EC091C91}"/>
+    <hyperlink ref="F2" r:id="rId5" xr:uid="{8FECC006-8CE2-4C2C-B26F-4DFCB885C971}"/>
+    <hyperlink ref="F3" r:id="rId6" xr:uid="{07B7F3B9-7ED0-459D-A5AD-E62B86EC2810}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{0B9415A8-0910-4D36-87D4-8247C3737E6C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change in overlay workflow for Marine input file
</commit_message>
<xml_diff>
--- a/NEAP_Extent_DataOverlayMaster.xlsx
+++ b/NEAP_Extent_DataOverlayMaster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/new298_csiro_au/Documents/Code/Python/NEAP/ecosystem-typology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC42371B-4E02-430B-B40A-B4CDED01A5D4}"/>
+  <xr:revisionPtr revIDLastSave="152" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E581F12-6D8A-420C-B1FF-DCE392DE9864}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2790" yWindow="3435" windowWidth="21600" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="62">
   <si>
     <t>Crosswalk</t>
   </si>
@@ -48,12 +48,6 @@
     <t>Complete</t>
   </si>
   <si>
-    <t>Natural Values Ecosystems</t>
-  </si>
-  <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Marine\NVE-Benthic\NESP-MERI_Natural_Values_Ecosystems.tif</t>
-  </si>
-  <si>
     <t>250m</t>
   </si>
   <si>
@@ -114,9 +108,6 @@
     <t>Complete. To be updated with edits from Anna and Suzanne</t>
   </si>
   <si>
-    <t>ALUM v8</t>
-  </si>
-  <si>
     <t>BSU</t>
   </si>
   <si>
@@ -199,6 +190,27 @@
   </si>
   <si>
     <t>ENVIRONMNT</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\Marine_Benthic.tif</t>
+  </si>
+  <si>
+    <t>Marine</t>
+  </si>
+  <si>
+    <t>ALUM 2010</t>
+  </si>
+  <si>
+    <t>ALUM 2015</t>
+  </si>
+  <si>
+    <t>ALUM 2020</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\ABARES_Land_use_of_Australia_2020_21_prerelease_20240712\ABARES_Land_use_of_Australia_2020_21_20240712\NLUM_v7p_ALUMV8_250m_2020_21_alb.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\NEAP_NLUM_2020-21_EPSG3577_250m.tif</t>
   </si>
 </sst>
 </file>
@@ -536,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,16 +572,16 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -578,16 +590,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>0</v>
@@ -598,69 +610,69 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J3" t="s">
         <v>4</v>
@@ -674,75 +686,75 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="K4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>12</v>
-      </c>
-      <c r="K4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L5" t="s">
         <v>6</v>
@@ -750,37 +762,37 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L6" t="s">
         <v>6</v>
@@ -788,78 +800,110 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" t="s">
         <v>26</v>
-      </c>
-      <c r="K7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L8" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -871,8 +915,9 @@
     <hyperlink ref="I2" r:id="rId5" xr:uid="{8FECC006-8CE2-4C2C-B26F-4DFCB885C971}"/>
     <hyperlink ref="I3" r:id="rId6" xr:uid="{07B7F3B9-7ED0-459D-A5AD-E62B86EC2810}"/>
     <hyperlink ref="I8" r:id="rId7" xr:uid="{0B9415A8-0910-4D36-87D4-8247C3737E6C}"/>
+    <hyperlink ref="I9" r:id="rId8" xr:uid="{8B471BD3-FA1D-4955-B103-79825EEF4FCB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update workflow file with object_labels
</commit_message>
<xml_diff>
--- a/NEAP_Extent_DataOverlayMaster.xlsx
+++ b/NEAP_Extent_DataOverlayMaster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/new298_csiro_au/Documents/Code/Python/NEAP/ecosystem-typology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="152" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E581F12-6D8A-420C-B1FF-DCE392DE9864}"/>
+  <xr:revisionPtr revIDLastSave="156" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF374819-5924-41AD-B2D7-C100A4B82D25}"/>
   <bookViews>
     <workbookView xWindow="2790" yWindow="3435" windowWidth="21600" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
   <si>
     <t>Crosswalk</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\NEAP_NLUM_2020-21_EPSG3577_250m.tif</t>
+  </si>
+  <si>
+    <t>TERTV8</t>
   </si>
 </sst>
 </file>
@@ -551,7 +554,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,7 +809,7 @@
         <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="D7" t="s">
         <v>49</v>
@@ -844,7 +847,7 @@
         <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="D8" t="s">
         <v>49</v>
@@ -879,7 +882,7 @@
         <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
update object_labels in workflow file
</commit_message>
<xml_diff>
--- a/NEAP_Extent_DataOverlayMaster.xlsx
+++ b/NEAP_Extent_DataOverlayMaster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/new298_csiro_au/Documents/Code/Python/NEAP/ecosystem-typology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF374819-5924-41AD-B2D7-C100A4B82D25}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1302405B-9504-42C5-8DF9-63941299CFCB}"/>
   <bookViews>
     <workbookView xWindow="2790" yWindow="3435" windowWidth="21600" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
   <si>
     <t>Crosswalk</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Complete. T4.4a (subject_label) narrow matches to be confirmed.</t>
   </si>
   <si>
-    <t>Terrestrial_NEAP</t>
-  </si>
-  <si>
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\NVIS_IUCNGET_DK_20240709.tif</t>
   </si>
   <si>
@@ -214,6 +211,12 @@
   </si>
   <si>
     <t>TERTV8</t>
+  </si>
+  <si>
+    <t>object_label</t>
+  </si>
+  <si>
+    <t>NVIS_NEAP</t>
   </si>
 </sst>
 </file>
@@ -554,7 +557,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,16 +578,16 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -593,16 +596,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>0</v>
@@ -613,16 +616,16 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -631,36 +634,36 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -672,10 +675,10 @@
         <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J3" t="s">
         <v>4</v>
@@ -689,31 +692,31 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J4" t="s">
         <v>10</v>
@@ -727,37 +730,37 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" t="s">
         <v>16</v>
-      </c>
-      <c r="K5" t="s">
-        <v>17</v>
       </c>
       <c r="L5" t="s">
         <v>6</v>
@@ -765,37 +768,37 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" t="s">
         <v>20</v>
-      </c>
-      <c r="K6" t="s">
-        <v>21</v>
       </c>
       <c r="L6" t="s">
         <v>6</v>
@@ -803,16 +806,16 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -821,36 +824,36 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" t="s">
         <v>24</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>25</v>
-      </c>
-      <c r="L7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -859,33 +862,33 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" t="s">
         <v>24</v>
-      </c>
-      <c r="K8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
         <v>59</v>
       </c>
-      <c r="B9" t="s">
-        <v>60</v>
-      </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -894,19 +897,19 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" t="s">
         <v>24</v>
-      </c>
-      <c r="K9" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to workflow control table with new BSU, NVIS and Marine input paths
</commit_message>
<xml_diff>
--- a/NEAP_Extent_DataOverlayMaster.xlsx
+++ b/NEAP_Extent_DataOverlayMaster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/new298_csiro_au/Documents/Code/Python/NEAP/ecosystem-typology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="160" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1302405B-9504-42C5-8DF9-63941299CFCB}"/>
+  <xr:revisionPtr revIDLastSave="166" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA167DFD-7541-4993-BA1D-D2570B8AC630}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="3435" windowWidth="21600" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7260" yWindow="1980" windowWidth="21792" windowHeight="14832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>Complete. T4.4a (subject_label) narrow matches to be confirmed.</t>
   </si>
   <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\NVIS_IUCNGET_DK_20240709.tif</t>
-  </si>
-  <si>
     <t>100m</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\BSU\NEAP_EcoExt_EPSG3577_250m.tif</t>
-  </si>
-  <si>
     <t>epsg:4326</t>
   </si>
   <si>
@@ -189,9 +183,6 @@
     <t>ENVIRONMNT</t>
   </si>
   <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\Marine_Benthic.tif</t>
-  </si>
-  <si>
     <t>Marine</t>
   </si>
   <si>
@@ -217,13 +208,22 @@
   </si>
   <si>
     <t>NVIS_NEAP</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\BSU\outputs\BSU_NEAP\BSU_NEAP_epsg3577_250m.tif</t>
+  </si>
+  <si>
+    <t>//fs1-cbr.nexus.csiro.au/{ev-neap}/work/extent/inputs/raw/Marine/NVE-Benthic/NESP-MERI_Natural_Values_Ecosystems_withVAT.tif</t>
+  </si>
+  <si>
+    <t>//fs1-cbr.nexus.csiro.au/{ev-neap}/work/extent/processing/NEAP_intermediate/NVIS_PRE1750_IUCNGET_DK_20240714.tif</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +247,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -269,10 +275,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -557,37 +570,37 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B9" sqref="B1:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="146.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="146.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="105.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="112.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="105.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="112.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -596,16 +609,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>0</v>
@@ -614,18 +627,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -634,36 +647,36 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -675,10 +688,10 @@
         <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J3" t="s">
         <v>4</v>
@@ -690,33 +703,33 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J4" t="s">
         <v>10</v>
@@ -728,94 +741,94 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" t="s">
         <v>15</v>
-      </c>
-      <c r="K5" t="s">
-        <v>16</v>
       </c>
       <c r="L5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" t="s">
         <v>19</v>
-      </c>
-      <c r="K6" t="s">
-        <v>20</v>
       </c>
       <c r="L6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -824,36 +837,36 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" t="s">
         <v>23</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>24</v>
       </c>
-      <c r="L7" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -862,33 +875,33 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" t="s">
         <v>23</v>
       </c>
-      <c r="K8" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
         <v>58</v>
       </c>
-      <c r="B9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" t="s">
-        <v>61</v>
-      </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -897,19 +910,19 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" t="s">
         <v>23</v>
-      </c>
-      <c r="K9" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -922,8 +935,9 @@
     <hyperlink ref="I3" r:id="rId6" xr:uid="{07B7F3B9-7ED0-459D-A5AD-E62B86EC2810}"/>
     <hyperlink ref="I8" r:id="rId7" xr:uid="{0B9415A8-0910-4D36-87D4-8247C3737E6C}"/>
     <hyperlink ref="I9" r:id="rId8" xr:uid="{8B471BD3-FA1D-4955-B103-79825EEF4FCB}"/>
+    <hyperlink ref="B2" r:id="rId9" xr:uid="{4AAD34BE-AFA6-4C42-98A5-31EBD33DB2C2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update Marine RAT subject_label
</commit_message>
<xml_diff>
--- a/NEAP_Extent_DataOverlayMaster.xlsx
+++ b/NEAP_Extent_DataOverlayMaster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/new298_csiro_au/Documents/Code/Python/NEAP/ecosystem-typology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA167DFD-7541-4993-BA1D-D2570B8AC630}"/>
+  <xr:revisionPtr revIDLastSave="168" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54C27DAB-D10E-4E25-8DF1-AA6DD78C48A4}"/>
   <bookViews>
-    <workbookView xWindow="7260" yWindow="1980" windowWidth="21792" windowHeight="14832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20712" yWindow="2448" windowWidth="21792" windowHeight="14832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
   <si>
     <t>Crosswalk</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>//fs1-cbr.nexus.csiro.au/{ev-neap}/work/extent/processing/NEAP_intermediate/NVIS_PRE1750_IUCNGET_DK_20240714.tif</t>
+  </si>
+  <si>
+    <t>subject_label</t>
   </si>
 </sst>
 </file>
@@ -570,7 +573,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B1:B9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -635,7 +638,7 @@
         <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
         <v>46</v>
@@ -673,7 +676,7 @@
         <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Update to workflow control table and change name for Lakes (lacustrine) crosswalk
</commit_message>
<xml_diff>
--- a/NEAP_Extent_DataOverlayMaster.xlsx
+++ b/NEAP_Extent_DataOverlayMaster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/new298_csiro_au/Documents/Code/Python/NEAP/ecosystem-typology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54C27DAB-D10E-4E25-8DF1-AA6DD78C48A4}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58FE8648-50E6-4980-855C-930E37572DCB}"/>
   <bookViews>
-    <workbookView xWindow="20712" yWindow="2448" windowWidth="21792" windowHeight="14832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10944" yWindow="1920" windowWidth="21792" windowHeight="14832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="59">
   <si>
     <t>Crosswalk</t>
   </si>
@@ -69,15 +69,6 @@
     <t>100m</t>
   </si>
   <si>
-    <t>Lakes-IUCNGET</t>
-  </si>
-  <si>
-    <t>https://github.com/CSIRO-enviro-informatics/ecosystem-typology/raw/main/crosswalks/Geofabric-IUCNGET/Lakes-IUCNGET.xlsx</t>
-  </si>
-  <si>
-    <t>Lakes_NEAP</t>
-  </si>
-  <si>
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\Lakes_NEAP.shp</t>
   </si>
   <si>
@@ -87,15 +78,9 @@
     <t>https://github.com/CSIRO-enviro-informatics/ecosystem-typology/raw/main/crosswalks/Estuarine-IUCNGET/Estuarine-IUCNGET.xlsx</t>
   </si>
   <si>
-    <t>OzEstuaries100K</t>
-  </si>
-  <si>
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\OzEstuariesRC100K\SeamapAus_NAT_CoastalGeomorph_OzEstuariesRC100KPolygon.shp</t>
   </si>
   <si>
-    <t>ALUM-IUCNGET</t>
-  </si>
-  <si>
     <t>https://github.com/CSIRO-enviro-informatics/ecosystem-typology/raw/main/crosswalks/ALUM-IUCNGET/ALUM-IUCNGET.xlsx</t>
   </si>
   <si>
@@ -105,9 +90,6 @@
     <t>BSU</t>
   </si>
   <si>
-    <t>Subject</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -129,24 +111,6 @@
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\NEAP_BSU_EPSG3577_250m.tif</t>
   </si>
   <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\NEAP_Marine_EPSG3577_250m.tif</t>
-  </si>
-  <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\NEAP_NVIS_EPSG3577_250m.tif</t>
-  </si>
-  <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\NEAP_Esturies_EPSG3577_250m.tif</t>
-  </si>
-  <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\NEAP_Lakes_EPSG3577_250m.tif</t>
-  </si>
-  <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\NEAP_NLUM_2010-11_EPSG3577_250m.tif</t>
-  </si>
-  <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\NEAP_NLUM_2015-16_EPSG3577_250m.tif</t>
-  </si>
-  <si>
     <t>ALL_TOUCHED</t>
   </si>
   <si>
@@ -183,33 +147,15 @@
     <t>ENVIRONMNT</t>
   </si>
   <si>
-    <t>Marine</t>
-  </si>
-  <si>
-    <t>ALUM 2010</t>
-  </si>
-  <si>
-    <t>ALUM 2015</t>
-  </si>
-  <si>
-    <t>ALUM 2020</t>
-  </si>
-  <si>
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\ABARES_Land_use_of_Australia_2020_21_prerelease_20240712\ABARES_Land_use_of_Australia_2020_21_20240712\NLUM_v7p_ALUMV8_250m_2020_21_alb.tif</t>
   </si>
   <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\NEAP_NLUM_2020-21_EPSG3577_250m.tif</t>
-  </si>
-  <si>
     <t>TERTV8</t>
   </si>
   <si>
     <t>object_label</t>
   </si>
   <si>
-    <t>NVIS_NEAP</t>
-  </si>
-  <si>
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\BSU\outputs\BSU_NEAP\BSU_NEAP_epsg3577_250m.tif</t>
   </si>
   <si>
@@ -220,6 +166,42 @@
   </si>
   <si>
     <t>subject_label</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\Marine_EPSG3577_250m.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\Terrestrial_EPSG3577_250m.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\Lacustrine_EPSG3577_250m.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\Estuarine_EPSG3577_250m.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\ALUM_2010_EPSG3577_250m.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\ALUM_2015_EPSG3577_250m.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\ALUM_2020_EPSG3577_250m.tif</t>
+  </si>
+  <si>
+    <t>ALUM_2010-IUCNGET</t>
+  </si>
+  <si>
+    <t>Lacustrine-IUCNGET</t>
+  </si>
+  <si>
+    <t>ALUM_2015-IUCNGET</t>
+  </si>
+  <si>
+    <t>ALUM_2020-IUCNGET</t>
+  </si>
+  <si>
+    <t>https://github.com/CSIRO-enviro-informatics/ecosystem-typology/raw/main/crosswalks/Geofabric-IUCNGET/Lacustrine-IUCNGET.xlsx</t>
   </si>
 </sst>
 </file>
@@ -570,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J7:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,23 +569,22 @@
     <col min="7" max="7" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="105.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="112.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.44140625" customWidth="1"/>
+    <col min="10" max="10" width="112.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -612,36 +593,33 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -650,36 +628,33 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -691,33 +666,30 @@
         <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
         <v>34</v>
-      </c>
-      <c r="J3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -729,109 +701,100 @@
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
         <v>35</v>
       </c>
-      <c r="J4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" t="s">
-        <v>12</v>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="K6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -840,36 +803,33 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="J7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="K7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -878,33 +838,30 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="J8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -913,19 +870,16 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J9" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -939,8 +893,9 @@
     <hyperlink ref="I8" r:id="rId7" xr:uid="{0B9415A8-0910-4D36-87D4-8247C3737E6C}"/>
     <hyperlink ref="I9" r:id="rId8" xr:uid="{8B471BD3-FA1D-4955-B103-79825EEF4FCB}"/>
     <hyperlink ref="B2" r:id="rId9" xr:uid="{4AAD34BE-AFA6-4C42-98A5-31EBD33DB2C2}"/>
+    <hyperlink ref="J5" r:id="rId10" xr:uid="{9D2ED58A-1BCA-4AFA-A7DB-AC11216EF831}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update workflow with new Laves crosswalk and small change to NVI crosswalk
</commit_message>
<xml_diff>
--- a/NEAP_Extent_DataOverlayMaster.xlsx
+++ b/NEAP_Extent_DataOverlayMaster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/new298_csiro_au/Documents/Code/Python/NEAP/ecosystem-typology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58FE8648-50E6-4980-855C-930E37572DCB}"/>
+  <xr:revisionPtr revIDLastSave="192" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0E9D513-AE19-4254-81E6-16964A41AA6B}"/>
   <bookViews>
-    <workbookView xWindow="10944" yWindow="1920" windowWidth="21792" windowHeight="14832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>100m</t>
   </si>
   <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\Lakes_NEAP.shp</t>
-  </si>
-  <si>
     <t>Estuarine-IUCNGET</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>https://github.com/CSIRO-enviro-informatics/ecosystem-typology/raw/main/crosswalks/Geofabric-IUCNGET/Lacustrine-IUCNGET.xlsx</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\Lakes_NEAP_20240723.shp</t>
   </si>
 </sst>
 </file>
@@ -554,14 +554,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J7:J8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="146.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="223" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.109375" customWidth="1"/>
@@ -575,16 +575,16 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -593,13 +593,13 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>0</v>
@@ -610,16 +610,16 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -628,19 +628,19 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -648,13 +648,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -666,10 +666,10 @@
         <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J3" t="s">
         <v>5</v>
@@ -683,13 +683,13 @@
         <v>10</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -701,10 +701,10 @@
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J4" t="s">
         <v>11</v>
@@ -715,34 +715,34 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
+        <v>54</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K5" t="s">
         <v>6</v>
@@ -750,34 +750,34 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J6" t="s">
-        <v>16</v>
       </c>
       <c r="K6" t="s">
         <v>6</v>
@@ -785,16 +785,16 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -803,33 +803,33 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" t="s">
         <v>18</v>
-      </c>
-      <c r="K7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -838,30 +838,30 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
         <v>40</v>
       </c>
-      <c r="C9" t="s">
-        <v>41</v>
-      </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -870,16 +870,16 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -894,8 +894,9 @@
     <hyperlink ref="I9" r:id="rId8" xr:uid="{8B471BD3-FA1D-4955-B103-79825EEF4FCB}"/>
     <hyperlink ref="B2" r:id="rId9" xr:uid="{4AAD34BE-AFA6-4C42-98A5-31EBD33DB2C2}"/>
     <hyperlink ref="J5" r:id="rId10" xr:uid="{9D2ED58A-1BCA-4AFA-A7DB-AC11216EF831}"/>
+    <hyperlink ref="B5" r:id="rId11" xr:uid="{6D271174-0A26-4C2B-8A49-23E0D84CB50C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update to workflow with links to latest ALUM 2020 data
</commit_message>
<xml_diff>
--- a/NEAP_Extent_DataOverlayMaster.xlsx
+++ b/NEAP_Extent_DataOverlayMaster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/new298_csiro_au/Documents/Code/Python/NEAP/ecosystem-typology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="192" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0E9D513-AE19-4254-81E6-16964A41AA6B}"/>
+  <xr:revisionPtr revIDLastSave="195" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BCFBB92-F273-4104-9AC4-2CE359B4B1A9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,9 +144,6 @@
     <t>ENVIRONMNT</t>
   </si>
   <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\ABARES_Land_use_of_Australia_2020_21_prerelease_20240712\ABARES_Land_use_of_Australia_2020_21_20240712\NLUM_v7p_ALUMV8_250m_2020_21_alb.tif</t>
-  </si>
-  <si>
     <t>TERTV8</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\Lakes_NEAP_20240723.shp</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\ABARES_Land_use_of_Australia_2020_21_prerelease2_20240724\ABARES_Land_use_of_Australia_2020_21_prerelease2_20240724\NLUM_v7p2_ALUMV8_250m_2020_21_alb.tif</t>
   </si>
 </sst>
 </file>
@@ -555,7 +555,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,7 +613,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -648,10 +648,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
         <v>33</v>
@@ -669,7 +669,7 @@
         <v>20</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J3" t="s">
         <v>5</v>
@@ -683,10 +683,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
         <v>33</v>
@@ -704,7 +704,7 @@
         <v>20</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J4" t="s">
         <v>11</v>
@@ -715,10 +715,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
@@ -739,10 +739,10 @@
         <v>27</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K5" t="s">
         <v>6</v>
@@ -774,7 +774,7 @@
         <v>27</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J6" t="s">
         <v>15</v>
@@ -785,13 +785,13 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
         <v>33</v>
@@ -809,7 +809,7 @@
         <v>20</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J7" t="s">
         <v>17</v>
@@ -820,13 +820,13 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
         <v>33</v>
@@ -844,7 +844,7 @@
         <v>20</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J8" t="s">
         <v>17</v>
@@ -852,13 +852,13 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
         <v>39</v>
-      </c>
-      <c r="C9" t="s">
-        <v>40</v>
       </c>
       <c r="D9" t="s">
         <v>33</v>
@@ -876,7 +876,7 @@
         <v>20</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J9" t="s">
         <v>17</v>

</xml_diff>